<commit_message>
modification des fichiers élèves
</commit_message>
<xml_diff>
--- a/Palmares/fichier excel/aggregats_ecoles_KASAI_CENTRAL12022.xlsx
+++ b/Palmares/fichier excel/aggregats_ecoles_KASAI_CENTRAL12022.xlsx
@@ -1,15 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Famille\OneDrive\Documents\GitHub\Projet-tutore\Palmares\fichier excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7790714-10A3-439C-A2D2-EB985D85475F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Écoles" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -2611,8 +2630,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2649,34 +2668,42 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="AggregatsEcoles" displayName="AggregatsEcoles" ref="A1:L516" totalsRowShown="0">
-  <autoFilter ref="A1:L516"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="AggregatsEcoles" displayName="AggregatsEcoles" ref="A1:L516" totalsRowShown="0">
+  <autoFilter ref="A1:L516" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="CodeEcole"/>
-    <tableColumn id="2" name="Ecole"/>
-    <tableColumn id="3" name="ProvinceEduc"/>
-    <tableColumn id="4" name="Annee"/>
-    <tableColumn id="5" name="CodeOption"/>
-    <tableColumn id="6" name="Option"/>
-    <tableColumn id="7" name="PartTot"/>
-    <tableColumn id="8" name="PartH"/>
-    <tableColumn id="9" name="PartF"/>
-    <tableColumn id="10" name="ReussTot"/>
-    <tableColumn id="11" name="ReussH"/>
-    <tableColumn id="12" name="ReussF"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="CodeEcole"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Ecole"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="ProvinceEduc"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Annee"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="CodeOption"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Option"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="PartTot"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="PartH"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="PartF"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="ReussTot"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="ReussH"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="ReussF"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2714,7 +2741,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -2748,6 +2775,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -2782,9 +2810,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2957,26 +2986,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L516"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:L1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" customWidth="1"/>
-    <col min="8" max="9" width="12.7109375" customWidth="1"/>
-    <col min="10" max="10" width="14.7109375" customWidth="1"/>
-    <col min="11" max="12" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1"/>
+    <col min="8" max="9" width="12.6640625" customWidth="1"/>
+    <col min="10" max="10" width="14.6640625" customWidth="1"/>
+    <col min="11" max="12" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>852</v>
       </c>
@@ -3014,7 +3045,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3052,7 +3083,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -3090,7 +3121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -3125,7 +3156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -3163,7 +3194,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -3201,7 +3232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -3239,7 +3270,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -3277,7 +3308,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -3312,7 +3343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -3347,7 +3378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -3382,7 +3413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -3420,7 +3451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -3458,7 +3489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -3493,7 +3524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -3528,7 +3559,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -3566,7 +3597,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -3604,7 +3635,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -3642,7 +3673,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -3680,7 +3711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -3718,7 +3749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -3756,7 +3787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -3794,7 +3825,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -3832,7 +3863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -3870,7 +3901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -3908,7 +3939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -3946,7 +3977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -3984,7 +4015,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -4019,7 +4050,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -4057,7 +4088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -4095,7 +4126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -4133,7 +4164,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -4171,7 +4202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -4209,7 +4240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -4247,7 +4278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -4285,7 +4316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -4323,7 +4354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -4361,7 +4392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -4399,7 +4430,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -4437,7 +4468,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -4475,7 +4506,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -4513,7 +4544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -4551,7 +4582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -4589,7 +4620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:12">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -4627,7 +4658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:12">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -4665,7 +4696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:12">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -4703,7 +4734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:12">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -4741,7 +4772,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="48" spans="1:12">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -4779,7 +4810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:12">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -4817,7 +4848,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="50" spans="1:12">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -4855,7 +4886,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="51" spans="1:12">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -4890,7 +4921,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:12">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -4928,7 +4959,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:12">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>51</v>
       </c>
@@ -4966,7 +4997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:12">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -5004,7 +5035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:12">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -5042,7 +5073,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:12">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>54</v>
       </c>
@@ -5080,7 +5111,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="57" spans="1:12">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -5118,7 +5149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:12">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>56</v>
       </c>
@@ -5153,7 +5184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:12">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>57</v>
       </c>
@@ -5191,7 +5222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:12">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>58</v>
       </c>
@@ -5226,7 +5257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:12">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>59</v>
       </c>
@@ -5264,7 +5295,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:12">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>60</v>
       </c>
@@ -5302,7 +5333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:12">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>61</v>
       </c>
@@ -5337,7 +5368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:12">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>62</v>
       </c>
@@ -5375,7 +5406,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:12">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>63</v>
       </c>
@@ -5413,7 +5444,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="66" spans="1:12">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>64</v>
       </c>
@@ -5451,7 +5482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:12">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>65</v>
       </c>
@@ -5486,7 +5517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:12">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>66</v>
       </c>
@@ -5524,7 +5555,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:12">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>67</v>
       </c>
@@ -5562,7 +5593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:12">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>68</v>
       </c>
@@ -5600,7 +5631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:12">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>69</v>
       </c>
@@ -5638,7 +5669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:12">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>70</v>
       </c>
@@ -5676,7 +5707,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="73" spans="1:12">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>71</v>
       </c>
@@ -5714,7 +5745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:12">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>72</v>
       </c>
@@ -5749,7 +5780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:12">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>73</v>
       </c>
@@ -5787,7 +5818,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="76" spans="1:12">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>74</v>
       </c>
@@ -5825,7 +5856,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="1:12">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>75</v>
       </c>
@@ -5860,7 +5891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:12">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>76</v>
       </c>
@@ -5895,7 +5926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:12">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>77</v>
       </c>
@@ -5930,7 +5961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:12">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>78</v>
       </c>
@@ -5968,7 +5999,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:12">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>79</v>
       </c>
@@ -6006,7 +6037,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="82" spans="1:12">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>80</v>
       </c>
@@ -6044,7 +6075,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="1:12">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>81</v>
       </c>
@@ -6082,7 +6113,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:12">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>82</v>
       </c>
@@ -6120,7 +6151,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:12">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>83</v>
       </c>
@@ -6155,7 +6186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:12">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>84</v>
       </c>
@@ -6193,7 +6224,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="87" spans="1:12">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>85</v>
       </c>
@@ -6231,7 +6262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:12">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>86</v>
       </c>
@@ -6269,7 +6300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:12">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>87</v>
       </c>
@@ -6307,7 +6338,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:12">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>88</v>
       </c>
@@ -6345,7 +6376,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="1:12">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>89</v>
       </c>
@@ -6383,7 +6414,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:12">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>90</v>
       </c>
@@ -6421,7 +6452,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:12">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>91</v>
       </c>
@@ -6459,7 +6490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:12">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>92</v>
       </c>
@@ -6497,7 +6528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:12">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>93</v>
       </c>
@@ -6535,7 +6566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:12">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>94</v>
       </c>
@@ -6573,7 +6604,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:12">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>95</v>
       </c>
@@ -6611,7 +6642,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="98" spans="1:12">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>96</v>
       </c>
@@ -6649,7 +6680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:12">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>97</v>
       </c>
@@ -6684,7 +6715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:12">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>98</v>
       </c>
@@ -6722,7 +6753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:12">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>99</v>
       </c>
@@ -6760,7 +6791,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="102" spans="1:12">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>100</v>
       </c>
@@ -6798,7 +6829,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="103" spans="1:12">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>101</v>
       </c>
@@ -6836,7 +6867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:12">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>102</v>
       </c>
@@ -6874,7 +6905,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="105" spans="1:12">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>103</v>
       </c>
@@ -6909,7 +6940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:12">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>104</v>
       </c>
@@ -6944,7 +6975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:12">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>105</v>
       </c>
@@ -6979,7 +7010,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="108" spans="1:12">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>106</v>
       </c>
@@ -7014,7 +7045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:12">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>107</v>
       </c>
@@ -7049,7 +7080,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="110" spans="1:12">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>108</v>
       </c>
@@ -7084,7 +7115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:12">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>109</v>
       </c>
@@ -7122,7 +7153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:12">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>110</v>
       </c>
@@ -7160,7 +7191,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="113" spans="1:12">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>111</v>
       </c>
@@ -7195,7 +7226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:12">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>112</v>
       </c>
@@ -7230,7 +7261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:12">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>113</v>
       </c>
@@ -7265,7 +7296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:12">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>114</v>
       </c>
@@ -7300,7 +7331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:12">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>115</v>
       </c>
@@ -7335,7 +7366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:12">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>116</v>
       </c>
@@ -7370,7 +7401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:12">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>117</v>
       </c>
@@ -7408,7 +7439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:12">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>118</v>
       </c>
@@ -7446,7 +7477,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="121" spans="1:12">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>119</v>
       </c>
@@ -7484,7 +7515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:12">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>120</v>
       </c>
@@ -7519,7 +7550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:12">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>121</v>
       </c>
@@ -7554,7 +7585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:12">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>122</v>
       </c>
@@ -7589,7 +7620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:12">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>123</v>
       </c>
@@ -7627,7 +7658,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="126" spans="1:12">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>124</v>
       </c>
@@ -7665,7 +7696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:12">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>125</v>
       </c>
@@ -7703,7 +7734,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="128" spans="1:12">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>126</v>
       </c>
@@ -7738,7 +7769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:12">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>127</v>
       </c>
@@ -7773,7 +7804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:12">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>128</v>
       </c>
@@ -7811,7 +7842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:12">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>129</v>
       </c>
@@ -7849,7 +7880,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="132" spans="1:12">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>130</v>
       </c>
@@ -7884,7 +7915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:12">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>131</v>
       </c>
@@ -7922,7 +7953,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="134" spans="1:12">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>132</v>
       </c>
@@ -7960,7 +7991,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="135" spans="1:12">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>133</v>
       </c>
@@ -7998,7 +8029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:12">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>134</v>
       </c>
@@ -8036,7 +8067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:12">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>135</v>
       </c>
@@ -8074,7 +8105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:12">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>136</v>
       </c>
@@ -8112,7 +8143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:12">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>137</v>
       </c>
@@ -8150,7 +8181,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="140" spans="1:12">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>138</v>
       </c>
@@ -8188,7 +8219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:12">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>139</v>
       </c>
@@ -8223,7 +8254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:12">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>140</v>
       </c>
@@ -8258,7 +8289,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="143" spans="1:12">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>141</v>
       </c>
@@ -8293,7 +8324,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="144" spans="1:12">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>142</v>
       </c>
@@ -8331,7 +8362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:12">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>143</v>
       </c>
@@ -8366,7 +8397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:12">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>144</v>
       </c>
@@ -8404,7 +8435,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="147" spans="1:12">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>145</v>
       </c>
@@ -8442,7 +8473,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="148" spans="1:12">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>146</v>
       </c>
@@ -8480,7 +8511,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="149" spans="1:12">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>147</v>
       </c>
@@ -8518,7 +8549,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="150" spans="1:12">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>148</v>
       </c>
@@ -8556,7 +8587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:12">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>149</v>
       </c>
@@ -8591,7 +8622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:12">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>150</v>
       </c>
@@ -8626,7 +8657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:12">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>151</v>
       </c>
@@ -8661,7 +8692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:12">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>152</v>
       </c>
@@ -8696,7 +8727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:12">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>153</v>
       </c>
@@ -8731,7 +8762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:12">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>154</v>
       </c>
@@ -8769,7 +8800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:12">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>155</v>
       </c>
@@ -8807,7 +8838,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="158" spans="1:12">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>156</v>
       </c>
@@ -8845,7 +8876,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="159" spans="1:12">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>157</v>
       </c>
@@ -8880,7 +8911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:12">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>158</v>
       </c>
@@ -8918,7 +8949,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="161" spans="1:12">
+    <row r="161" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>159</v>
       </c>
@@ -8956,7 +8987,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="162" spans="1:12">
+    <row r="162" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>160</v>
       </c>
@@ -8991,7 +9022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:12">
+    <row r="163" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>161</v>
       </c>
@@ -9029,7 +9060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:12">
+    <row r="164" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>162</v>
       </c>
@@ -9067,7 +9098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:12">
+    <row r="165" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>163</v>
       </c>
@@ -9105,7 +9136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:12">
+    <row r="166" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>164</v>
       </c>
@@ -9143,7 +9174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:12">
+    <row r="167" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>165</v>
       </c>
@@ -9181,7 +9212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:12">
+    <row r="168" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>166</v>
       </c>
@@ -9219,7 +9250,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="169" spans="1:12">
+    <row r="169" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>167</v>
       </c>
@@ -9257,7 +9288,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="170" spans="1:12">
+    <row r="170" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>168</v>
       </c>
@@ -9292,7 +9323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:12">
+    <row r="171" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>169</v>
       </c>
@@ -9327,7 +9358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:12">
+    <row r="172" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>170</v>
       </c>
@@ -9365,7 +9396,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="173" spans="1:12">
+    <row r="173" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>171</v>
       </c>
@@ -9403,7 +9434,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="174" spans="1:12">
+    <row r="174" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>172</v>
       </c>
@@ -9438,7 +9469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:12">
+    <row r="175" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>173</v>
       </c>
@@ -9473,7 +9504,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="176" spans="1:12">
+    <row r="176" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>174</v>
       </c>
@@ -9511,7 +9542,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="177" spans="1:12">
+    <row r="177" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>175</v>
       </c>
@@ -9549,7 +9580,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="178" spans="1:12">
+    <row r="178" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>176</v>
       </c>
@@ -9584,7 +9615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:12">
+    <row r="179" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>177</v>
       </c>
@@ -9619,7 +9650,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="180" spans="1:12">
+    <row r="180" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>178</v>
       </c>
@@ -9654,7 +9685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:12">
+    <row r="181" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>179</v>
       </c>
@@ -9692,7 +9723,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="182" spans="1:12">
+    <row r="182" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>180</v>
       </c>
@@ -9730,7 +9761,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="183" spans="1:12">
+    <row r="183" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>181</v>
       </c>
@@ -9768,7 +9799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:12">
+    <row r="184" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>182</v>
       </c>
@@ -9806,7 +9837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:12">
+    <row r="185" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>183</v>
       </c>
@@ -9841,7 +9872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:12">
+    <row r="186" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>184</v>
       </c>
@@ -9876,7 +9907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:12">
+    <row r="187" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>185</v>
       </c>
@@ -9914,7 +9945,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="188" spans="1:12">
+    <row r="188" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>186</v>
       </c>
@@ -9952,7 +9983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:12">
+    <row r="189" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>187</v>
       </c>
@@ -9990,7 +10021,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="190" spans="1:12">
+    <row r="190" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>188</v>
       </c>
@@ -10028,7 +10059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:12">
+    <row r="191" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>189</v>
       </c>
@@ -10066,7 +10097,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="192" spans="1:12">
+    <row r="192" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>190</v>
       </c>
@@ -10104,7 +10135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:12">
+    <row r="193" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>191</v>
       </c>
@@ -10139,7 +10170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:12">
+    <row r="194" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>192</v>
       </c>
@@ -10174,7 +10205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:12">
+    <row r="195" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>193</v>
       </c>
@@ -10209,7 +10240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:12">
+    <row r="196" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>194</v>
       </c>
@@ -10244,7 +10275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:12">
+    <row r="197" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>195</v>
       </c>
@@ -10279,7 +10310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:12">
+    <row r="198" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>196</v>
       </c>
@@ -10317,7 +10348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:12">
+    <row r="199" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>197</v>
       </c>
@@ -10355,7 +10386,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="200" spans="1:12">
+    <row r="200" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>198</v>
       </c>
@@ -10393,7 +10424,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="201" spans="1:12">
+    <row r="201" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>199</v>
       </c>
@@ -10431,7 +10462,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="202" spans="1:12">
+    <row r="202" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>200</v>
       </c>
@@ -10469,7 +10500,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="203" spans="1:12">
+    <row r="203" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>201</v>
       </c>
@@ -10504,7 +10535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:12">
+    <row r="204" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>202</v>
       </c>
@@ -10542,7 +10573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:12">
+    <row r="205" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>203</v>
       </c>
@@ -10580,7 +10611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:12">
+    <row r="206" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>204</v>
       </c>
@@ -10618,7 +10649,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="207" spans="1:12">
+    <row r="207" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>205</v>
       </c>
@@ -10656,7 +10687,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="208" spans="1:12">
+    <row r="208" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>206</v>
       </c>
@@ -10694,7 +10725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:12">
+    <row r="209" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>207</v>
       </c>
@@ -10729,7 +10760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:12">
+    <row r="210" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>208</v>
       </c>
@@ -10764,7 +10795,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="211" spans="1:12">
+    <row r="211" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>209</v>
       </c>
@@ -10802,7 +10833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:12">
+    <row r="212" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>210</v>
       </c>
@@ -10837,7 +10868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:12">
+    <row r="213" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>211</v>
       </c>
@@ -10875,7 +10906,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="214" spans="1:12">
+    <row r="214" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>212</v>
       </c>
@@ -10913,7 +10944,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="215" spans="1:12">
+    <row r="215" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>213</v>
       </c>
@@ -10951,7 +10982,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="216" spans="1:12">
+    <row r="216" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>214</v>
       </c>
@@ -10989,7 +11020,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="217" spans="1:12">
+    <row r="217" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>215</v>
       </c>
@@ -11027,7 +11058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:12">
+    <row r="218" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>216</v>
       </c>
@@ -11065,7 +11096,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="219" spans="1:12">
+    <row r="219" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>217</v>
       </c>
@@ -11103,7 +11134,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="220" spans="1:12">
+    <row r="220" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>218</v>
       </c>
@@ -11141,7 +11172,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="221" spans="1:12">
+    <row r="221" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>219</v>
       </c>
@@ -11176,7 +11207,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="222" spans="1:12">
+    <row r="222" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>220</v>
       </c>
@@ -11211,7 +11242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:12">
+    <row r="223" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>221</v>
       </c>
@@ -11246,7 +11277,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="224" spans="1:12">
+    <row r="224" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>222</v>
       </c>
@@ -11284,7 +11315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="225" spans="1:12">
+    <row r="225" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>223</v>
       </c>
@@ -11322,7 +11353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:12">
+    <row r="226" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>224</v>
       </c>
@@ -11357,7 +11388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:12">
+    <row r="227" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>225</v>
       </c>
@@ -11395,7 +11426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:12">
+    <row r="228" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>226</v>
       </c>
@@ -11433,7 +11464,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="229" spans="1:12">
+    <row r="229" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>227</v>
       </c>
@@ -11471,7 +11502,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="230" spans="1:12">
+    <row r="230" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>228</v>
       </c>
@@ -11506,7 +11537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:12">
+    <row r="231" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>229</v>
       </c>
@@ -11541,7 +11572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:12">
+    <row r="232" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>230</v>
       </c>
@@ -11579,7 +11610,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="233" spans="1:12">
+    <row r="233" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>231</v>
       </c>
@@ -11617,7 +11648,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="234" spans="1:12">
+    <row r="234" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>232</v>
       </c>
@@ -11655,7 +11686,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="235" spans="1:12">
+    <row r="235" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>233</v>
       </c>
@@ -11693,7 +11724,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="236" spans="1:12">
+    <row r="236" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>234</v>
       </c>
@@ -11728,7 +11759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:12">
+    <row r="237" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>235</v>
       </c>
@@ -11763,7 +11794,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="238" spans="1:12">
+    <row r="238" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>236</v>
       </c>
@@ -11801,7 +11832,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="239" spans="1:12">
+    <row r="239" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>237</v>
       </c>
@@ -11839,7 +11870,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="240" spans="1:12">
+    <row r="240" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>238</v>
       </c>
@@ -11877,7 +11908,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="241" spans="1:12">
+    <row r="241" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>239</v>
       </c>
@@ -11915,7 +11946,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="242" spans="1:12">
+    <row r="242" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>240</v>
       </c>
@@ -11950,7 +11981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:12">
+    <row r="243" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>241</v>
       </c>
@@ -11985,7 +12016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:12">
+    <row r="244" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>242</v>
       </c>
@@ -12020,7 +12051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:12">
+    <row r="245" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>243</v>
       </c>
@@ -12058,7 +12089,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="246" spans="1:12">
+    <row r="246" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>244</v>
       </c>
@@ -12096,7 +12127,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="247" spans="1:12">
+    <row r="247" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>245</v>
       </c>
@@ -12134,7 +12165,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="248" spans="1:12">
+    <row r="248" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>246</v>
       </c>
@@ -12172,7 +12203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:12">
+    <row r="249" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>247</v>
       </c>
@@ -12210,7 +12241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="250" spans="1:12">
+    <row r="250" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>248</v>
       </c>
@@ -12248,7 +12279,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="251" spans="1:12">
+    <row r="251" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>249</v>
       </c>
@@ -12286,7 +12317,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="252" spans="1:12">
+    <row r="252" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>250</v>
       </c>
@@ -12321,7 +12352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:12">
+    <row r="253" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>251</v>
       </c>
@@ -12359,7 +12390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:12">
+    <row r="254" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>252</v>
       </c>
@@ -12397,7 +12428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:12">
+    <row r="255" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>253</v>
       </c>
@@ -12435,7 +12466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:12">
+    <row r="256" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>254</v>
       </c>
@@ -12473,7 +12504,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="257" spans="1:12">
+    <row r="257" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>255</v>
       </c>
@@ -12511,7 +12542,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="258" spans="1:12">
+    <row r="258" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>256</v>
       </c>
@@ -12549,7 +12580,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="259" spans="1:12">
+    <row r="259" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>257</v>
       </c>
@@ -12587,7 +12618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:12">
+    <row r="260" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>258</v>
       </c>
@@ -12625,7 +12656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:12">
+    <row r="261" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>259</v>
       </c>
@@ -12663,7 +12694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:12">
+    <row r="262" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>260</v>
       </c>
@@ -12701,7 +12732,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="263" spans="1:12">
+    <row r="263" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>261</v>
       </c>
@@ -12739,7 +12770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:12">
+    <row r="264" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>262</v>
       </c>
@@ -12774,7 +12805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:12">
+    <row r="265" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>263</v>
       </c>
@@ -12812,7 +12843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:12">
+    <row r="266" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>264</v>
       </c>
@@ -12850,7 +12881,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="267" spans="1:12">
+    <row r="267" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>265</v>
       </c>
@@ -12888,7 +12919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:12">
+    <row r="268" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>266</v>
       </c>
@@ -12926,7 +12957,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="269" spans="1:12">
+    <row r="269" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>267</v>
       </c>
@@ -12964,7 +12995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:12">
+    <row r="270" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>268</v>
       </c>
@@ -13002,7 +13033,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="271" spans="1:12">
+    <row r="271" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>269</v>
       </c>
@@ -13040,7 +13071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="272" spans="1:12">
+    <row r="272" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>270</v>
       </c>
@@ -13075,7 +13106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:12">
+    <row r="273" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>271</v>
       </c>
@@ -13110,7 +13141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:12">
+    <row r="274" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>272</v>
       </c>
@@ -13148,7 +13179,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="275" spans="1:12">
+    <row r="275" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>273</v>
       </c>
@@ -13186,7 +13217,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="276" spans="1:12">
+    <row r="276" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>274</v>
       </c>
@@ -13224,7 +13255,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="277" spans="1:12">
+    <row r="277" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>275</v>
       </c>
@@ -13262,7 +13293,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="278" spans="1:12">
+    <row r="278" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>276</v>
       </c>
@@ -13300,7 +13331,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="279" spans="1:12">
+    <row r="279" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>277</v>
       </c>
@@ -13335,7 +13366,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="280" spans="1:12">
+    <row r="280" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>278</v>
       </c>
@@ -13370,7 +13401,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="281" spans="1:12">
+    <row r="281" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>279</v>
       </c>
@@ -13405,7 +13436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:12">
+    <row r="282" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>280</v>
       </c>
@@ -13443,7 +13474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="1:12">
+    <row r="283" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>281</v>
       </c>
@@ -13481,7 +13512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:12">
+    <row r="284" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>282</v>
       </c>
@@ -13519,7 +13550,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="285" spans="1:12">
+    <row r="285" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>283</v>
       </c>
@@ -13557,7 +13588,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="286" spans="1:12">
+    <row r="286" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>284</v>
       </c>
@@ -13595,7 +13626,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="287" spans="1:12">
+    <row r="287" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>285</v>
       </c>
@@ -13630,7 +13661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:12">
+    <row r="288" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>286</v>
       </c>
@@ -13668,7 +13699,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="289" spans="1:12">
+    <row r="289" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>287</v>
       </c>
@@ -13706,7 +13737,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="290" spans="1:12">
+    <row r="290" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>288</v>
       </c>
@@ -13744,7 +13775,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="291" spans="1:12">
+    <row r="291" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>289</v>
       </c>
@@ -13782,7 +13813,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="292" spans="1:12">
+    <row r="292" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>290</v>
       </c>
@@ -13820,7 +13851,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="293" spans="1:12">
+    <row r="293" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>291</v>
       </c>
@@ -13858,7 +13889,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="294" spans="1:12">
+    <row r="294" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>292</v>
       </c>
@@ -13896,7 +13927,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="295" spans="1:12">
+    <row r="295" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>293</v>
       </c>
@@ -13931,7 +13962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:12">
+    <row r="296" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>294</v>
       </c>
@@ -13969,7 +14000,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="297" spans="1:12">
+    <row r="297" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>295</v>
       </c>
@@ -14007,7 +14038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="1:12">
+    <row r="298" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>296</v>
       </c>
@@ -14045,7 +14076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="299" spans="1:12">
+    <row r="299" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>297</v>
       </c>
@@ -14083,7 +14114,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="300" spans="1:12">
+    <row r="300" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>298</v>
       </c>
@@ -14121,7 +14152,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="301" spans="1:12">
+    <row r="301" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>299</v>
       </c>
@@ -14159,7 +14190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="302" spans="1:12">
+    <row r="302" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
         <v>300</v>
       </c>
@@ -14197,7 +14228,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="303" spans="1:12">
+    <row r="303" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
         <v>301</v>
       </c>
@@ -14235,7 +14266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="304" spans="1:12">
+    <row r="304" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
         <v>302</v>
       </c>
@@ -14273,7 +14304,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="305" spans="1:12">
+    <row r="305" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
         <v>303</v>
       </c>
@@ -14311,7 +14342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="306" spans="1:12">
+    <row r="306" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
         <v>304</v>
       </c>
@@ -14349,7 +14380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="307" spans="1:12">
+    <row r="307" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
         <v>305</v>
       </c>
@@ -14387,7 +14418,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="308" spans="1:12">
+    <row r="308" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
         <v>306</v>
       </c>
@@ -14425,7 +14456,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="309" spans="1:12">
+    <row r="309" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
         <v>307</v>
       </c>
@@ -14463,7 +14494,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="310" spans="1:12">
+    <row r="310" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
         <v>308</v>
       </c>
@@ -14498,7 +14529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="311" spans="1:12">
+    <row r="311" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
         <v>309</v>
       </c>
@@ -14533,7 +14564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="312" spans="1:12">
+    <row r="312" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
         <v>310</v>
       </c>
@@ -14571,7 +14602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="313" spans="1:12">
+    <row r="313" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
         <v>311</v>
       </c>
@@ -14609,7 +14640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="314" spans="1:12">
+    <row r="314" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
         <v>312</v>
       </c>
@@ -14647,7 +14678,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="315" spans="1:12">
+    <row r="315" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
         <v>313</v>
       </c>
@@ -14685,7 +14716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="316" spans="1:12">
+    <row r="316" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
         <v>314</v>
       </c>
@@ -14723,7 +14754,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="317" spans="1:12">
+    <row r="317" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
         <v>315</v>
       </c>
@@ -14761,7 +14792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="318" spans="1:12">
+    <row r="318" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
         <v>316</v>
       </c>
@@ -14799,7 +14830,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="319" spans="1:12">
+    <row r="319" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
         <v>317</v>
       </c>
@@ -14834,7 +14865,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="320" spans="1:12">
+    <row r="320" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
         <v>318</v>
       </c>
@@ -14869,7 +14900,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="321" spans="1:12">
+    <row r="321" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
         <v>319</v>
       </c>
@@ -14907,7 +14938,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="322" spans="1:12">
+    <row r="322" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
         <v>320</v>
       </c>
@@ -14945,7 +14976,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="323" spans="1:12">
+    <row r="323" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
         <v>321</v>
       </c>
@@ -14983,7 +15014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="324" spans="1:12">
+    <row r="324" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
         <v>322</v>
       </c>
@@ -15021,7 +15052,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="325" spans="1:12">
+    <row r="325" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
         <v>323</v>
       </c>
@@ -15059,7 +15090,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="326" spans="1:12">
+    <row r="326" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
         <v>324</v>
       </c>
@@ -15097,7 +15128,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="327" spans="1:12">
+    <row r="327" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
         <v>325</v>
       </c>
@@ -15135,7 +15166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="328" spans="1:12">
+    <row r="328" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
         <v>326</v>
       </c>
@@ -15173,7 +15204,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="329" spans="1:12">
+    <row r="329" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
         <v>327</v>
       </c>
@@ -15208,7 +15239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="330" spans="1:12">
+    <row r="330" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
         <v>328</v>
       </c>
@@ -15243,7 +15274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="331" spans="1:12">
+    <row r="331" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
         <v>329</v>
       </c>
@@ -15278,7 +15309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="332" spans="1:12">
+    <row r="332" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
         <v>330</v>
       </c>
@@ -15316,7 +15347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="333" spans="1:12">
+    <row r="333" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
         <v>331</v>
       </c>
@@ -15354,7 +15385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="334" spans="1:12">
+    <row r="334" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
         <v>332</v>
       </c>
@@ -15389,7 +15420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="335" spans="1:12">
+    <row r="335" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
         <v>333</v>
       </c>
@@ -15427,7 +15458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="336" spans="1:12">
+    <row r="336" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
         <v>334</v>
       </c>
@@ -15465,7 +15496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="337" spans="1:12">
+    <row r="337" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
         <v>335</v>
       </c>
@@ -15503,7 +15534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="338" spans="1:12">
+    <row r="338" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
         <v>336</v>
       </c>
@@ -15541,7 +15572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="339" spans="1:12">
+    <row r="339" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
         <v>337</v>
       </c>
@@ -15579,7 +15610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="340" spans="1:12">
+    <row r="340" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
         <v>338</v>
       </c>
@@ -15617,7 +15648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="341" spans="1:12">
+    <row r="341" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
         <v>339</v>
       </c>
@@ -15655,7 +15686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="342" spans="1:12">
+    <row r="342" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
         <v>340</v>
       </c>
@@ -15693,7 +15724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="343" spans="1:12">
+    <row r="343" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
         <v>341</v>
       </c>
@@ -15731,7 +15762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="344" spans="1:12">
+    <row r="344" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
         <v>342</v>
       </c>
@@ -15769,7 +15800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="345" spans="1:12">
+    <row r="345" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
         <v>343</v>
       </c>
@@ -15807,7 +15838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="346" spans="1:12">
+    <row r="346" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A346" t="s">
         <v>344</v>
       </c>
@@ -15845,7 +15876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="347" spans="1:12">
+    <row r="347" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
         <v>345</v>
       </c>
@@ -15883,7 +15914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="348" spans="1:12">
+    <row r="348" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
         <v>346</v>
       </c>
@@ -15921,7 +15952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="349" spans="1:12">
+    <row r="349" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
         <v>347</v>
       </c>
@@ -15959,7 +15990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="350" spans="1:12">
+    <row r="350" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A350" t="s">
         <v>348</v>
       </c>
@@ -15997,7 +16028,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="351" spans="1:12">
+    <row r="351" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
         <v>349</v>
       </c>
@@ -16035,7 +16066,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="352" spans="1:12">
+    <row r="352" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
         <v>350</v>
       </c>
@@ -16070,7 +16101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="353" spans="1:12">
+    <row r="353" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
         <v>351</v>
       </c>
@@ -16108,7 +16139,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="354" spans="1:12">
+    <row r="354" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
         <v>352</v>
       </c>
@@ -16146,7 +16177,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="355" spans="1:12">
+    <row r="355" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A355" t="s">
         <v>353</v>
       </c>
@@ -16184,7 +16215,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="356" spans="1:12">
+    <row r="356" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A356" t="s">
         <v>354</v>
       </c>
@@ -16219,7 +16250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="357" spans="1:12">
+    <row r="357" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
         <v>355</v>
       </c>
@@ -16254,7 +16285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="358" spans="1:12">
+    <row r="358" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A358" t="s">
         <v>356</v>
       </c>
@@ -16292,7 +16323,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="359" spans="1:12">
+    <row r="359" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A359" t="s">
         <v>357</v>
       </c>
@@ -16330,7 +16361,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="360" spans="1:12">
+    <row r="360" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A360" t="s">
         <v>358</v>
       </c>
@@ -16368,7 +16399,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="361" spans="1:12">
+    <row r="361" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A361" t="s">
         <v>359</v>
       </c>
@@ -16403,7 +16434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="362" spans="1:12">
+    <row r="362" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A362" t="s">
         <v>360</v>
       </c>
@@ -16438,7 +16469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="363" spans="1:12">
+    <row r="363" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A363" t="s">
         <v>361</v>
       </c>
@@ -16473,7 +16504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="364" spans="1:12">
+    <row r="364" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A364" t="s">
         <v>362</v>
       </c>
@@ -16511,7 +16542,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="365" spans="1:12">
+    <row r="365" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A365" t="s">
         <v>363</v>
       </c>
@@ -16549,7 +16580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="366" spans="1:12">
+    <row r="366" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A366" t="s">
         <v>364</v>
       </c>
@@ -16587,7 +16618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="367" spans="1:12">
+    <row r="367" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A367" t="s">
         <v>365</v>
       </c>
@@ -16625,7 +16656,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="368" spans="1:12">
+    <row r="368" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A368" t="s">
         <v>366</v>
       </c>
@@ -16663,7 +16694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="369" spans="1:12">
+    <row r="369" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A369" t="s">
         <v>367</v>
       </c>
@@ -16701,7 +16732,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="370" spans="1:12">
+    <row r="370" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A370" t="s">
         <v>368</v>
       </c>
@@ -16739,7 +16770,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="371" spans="1:12">
+    <row r="371" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A371" t="s">
         <v>369</v>
       </c>
@@ -16777,7 +16808,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="372" spans="1:12">
+    <row r="372" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A372" t="s">
         <v>370</v>
       </c>
@@ -16815,7 +16846,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="373" spans="1:12">
+    <row r="373" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A373" t="s">
         <v>371</v>
       </c>
@@ -16850,7 +16881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="374" spans="1:12">
+    <row r="374" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A374" t="s">
         <v>372</v>
       </c>
@@ -16888,7 +16919,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="375" spans="1:12">
+    <row r="375" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A375" t="s">
         <v>373</v>
       </c>
@@ -16926,7 +16957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="376" spans="1:12">
+    <row r="376" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A376" t="s">
         <v>374</v>
       </c>
@@ -16961,7 +16992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="377" spans="1:12">
+    <row r="377" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A377" t="s">
         <v>375</v>
       </c>
@@ -16999,7 +17030,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="378" spans="1:12">
+    <row r="378" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A378" t="s">
         <v>376</v>
       </c>
@@ -17037,7 +17068,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="379" spans="1:12">
+    <row r="379" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A379" t="s">
         <v>377</v>
       </c>
@@ -17075,7 +17106,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="380" spans="1:12">
+    <row r="380" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A380" t="s">
         <v>378</v>
       </c>
@@ -17113,7 +17144,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="381" spans="1:12">
+    <row r="381" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A381" t="s">
         <v>379</v>
       </c>
@@ -17151,7 +17182,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="382" spans="1:12">
+    <row r="382" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A382" t="s">
         <v>380</v>
       </c>
@@ -17186,7 +17217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="383" spans="1:12">
+    <row r="383" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A383" t="s">
         <v>381</v>
       </c>
@@ -17224,7 +17255,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="384" spans="1:12">
+    <row r="384" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A384" t="s">
         <v>382</v>
       </c>
@@ -17259,7 +17290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="385" spans="1:12">
+    <row r="385" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A385" t="s">
         <v>383</v>
       </c>
@@ -17294,7 +17325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="386" spans="1:12">
+    <row r="386" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A386" t="s">
         <v>384</v>
       </c>
@@ -17329,7 +17360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="387" spans="1:12">
+    <row r="387" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A387" t="s">
         <v>385</v>
       </c>
@@ -17367,7 +17398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="388" spans="1:12">
+    <row r="388" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A388" t="s">
         <v>386</v>
       </c>
@@ -17405,7 +17436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="389" spans="1:12">
+    <row r="389" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A389" t="s">
         <v>387</v>
       </c>
@@ -17443,7 +17474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="390" spans="1:12">
+    <row r="390" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A390" t="s">
         <v>388</v>
       </c>
@@ -17481,7 +17512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="391" spans="1:12">
+    <row r="391" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A391" t="s">
         <v>389</v>
       </c>
@@ -17519,7 +17550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="392" spans="1:12">
+    <row r="392" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A392" t="s">
         <v>390</v>
       </c>
@@ -17557,7 +17588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="393" spans="1:12">
+    <row r="393" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A393" t="s">
         <v>391</v>
       </c>
@@ -17592,7 +17623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="394" spans="1:12">
+    <row r="394" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A394" t="s">
         <v>392</v>
       </c>
@@ -17627,7 +17658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="395" spans="1:12">
+    <row r="395" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A395" t="s">
         <v>393</v>
       </c>
@@ -17665,7 +17696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="396" spans="1:12">
+    <row r="396" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A396" t="s">
         <v>394</v>
       </c>
@@ -17700,7 +17731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="397" spans="1:12">
+    <row r="397" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A397" t="s">
         <v>395</v>
       </c>
@@ -17738,7 +17769,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="398" spans="1:12">
+    <row r="398" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A398" t="s">
         <v>396</v>
       </c>
@@ -17776,7 +17807,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="399" spans="1:12">
+    <row r="399" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A399" t="s">
         <v>397</v>
       </c>
@@ -17814,7 +17845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="400" spans="1:12">
+    <row r="400" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A400" t="s">
         <v>398</v>
       </c>
@@ -17852,7 +17883,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="401" spans="1:12">
+    <row r="401" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A401" t="s">
         <v>399</v>
       </c>
@@ -17890,7 +17921,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="402" spans="1:12">
+    <row r="402" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A402" t="s">
         <v>400</v>
       </c>
@@ -17928,7 +17959,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="403" spans="1:12">
+    <row r="403" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A403" t="s">
         <v>401</v>
       </c>
@@ -17966,7 +17997,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="404" spans="1:12">
+    <row r="404" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A404" t="s">
         <v>402</v>
       </c>
@@ -18004,7 +18035,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="405" spans="1:12">
+    <row r="405" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A405" t="s">
         <v>403</v>
       </c>
@@ -18039,7 +18070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="406" spans="1:12">
+    <row r="406" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A406" t="s">
         <v>404</v>
       </c>
@@ -18074,7 +18105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="407" spans="1:12">
+    <row r="407" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A407" t="s">
         <v>405</v>
       </c>
@@ -18112,7 +18143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="408" spans="1:12">
+    <row r="408" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A408" t="s">
         <v>406</v>
       </c>
@@ -18150,7 +18181,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="409" spans="1:12">
+    <row r="409" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A409" t="s">
         <v>407</v>
       </c>
@@ -18188,7 +18219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="410" spans="1:12">
+    <row r="410" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A410" t="s">
         <v>408</v>
       </c>
@@ -18226,7 +18257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="411" spans="1:12">
+    <row r="411" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A411" t="s">
         <v>409</v>
       </c>
@@ -18264,7 +18295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="412" spans="1:12">
+    <row r="412" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A412" t="s">
         <v>410</v>
       </c>
@@ -18299,7 +18330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="413" spans="1:12">
+    <row r="413" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A413" t="s">
         <v>411</v>
       </c>
@@ -18337,7 +18368,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="414" spans="1:12">
+    <row r="414" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A414" t="s">
         <v>412</v>
       </c>
@@ -18375,7 +18406,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="415" spans="1:12">
+    <row r="415" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A415" t="s">
         <v>413</v>
       </c>
@@ -18413,7 +18444,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="416" spans="1:12">
+    <row r="416" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A416" t="s">
         <v>414</v>
       </c>
@@ -18451,7 +18482,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="417" spans="1:12">
+    <row r="417" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A417" t="s">
         <v>415</v>
       </c>
@@ -18489,7 +18520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="418" spans="1:12">
+    <row r="418" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A418" t="s">
         <v>416</v>
       </c>
@@ -18527,7 +18558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="419" spans="1:12">
+    <row r="419" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A419" t="s">
         <v>417</v>
       </c>
@@ -18565,7 +18596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="420" spans="1:12">
+    <row r="420" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A420" t="s">
         <v>418</v>
       </c>
@@ -18600,7 +18631,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="421" spans="1:12">
+    <row r="421" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A421" t="s">
         <v>419</v>
       </c>
@@ -18635,7 +18666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="422" spans="1:12">
+    <row r="422" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A422" t="s">
         <v>420</v>
       </c>
@@ -18670,7 +18701,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="423" spans="1:12">
+    <row r="423" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A423" t="s">
         <v>421</v>
       </c>
@@ -18708,7 +18739,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="424" spans="1:12">
+    <row r="424" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A424" t="s">
         <v>422</v>
       </c>
@@ -18746,7 +18777,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="425" spans="1:12">
+    <row r="425" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A425" t="s">
         <v>423</v>
       </c>
@@ -18784,7 +18815,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="426" spans="1:12">
+    <row r="426" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A426" t="s">
         <v>424</v>
       </c>
@@ -18822,7 +18853,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="427" spans="1:12">
+    <row r="427" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A427" t="s">
         <v>425</v>
       </c>
@@ -18857,7 +18888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="428" spans="1:12">
+    <row r="428" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A428" t="s">
         <v>426</v>
       </c>
@@ -18892,7 +18923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="429" spans="1:12">
+    <row r="429" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A429" t="s">
         <v>427</v>
       </c>
@@ -18930,7 +18961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="430" spans="1:12">
+    <row r="430" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A430" t="s">
         <v>428</v>
       </c>
@@ -18968,7 +18999,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="431" spans="1:12">
+    <row r="431" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A431" t="s">
         <v>429</v>
       </c>
@@ -19006,7 +19037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="432" spans="1:12">
+    <row r="432" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A432" t="s">
         <v>430</v>
       </c>
@@ -19044,7 +19075,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="433" spans="1:12">
+    <row r="433" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A433" t="s">
         <v>431</v>
       </c>
@@ -19082,7 +19113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="434" spans="1:12">
+    <row r="434" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A434" t="s">
         <v>432</v>
       </c>
@@ -19120,7 +19151,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="435" spans="1:12">
+    <row r="435" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A435" t="s">
         <v>433</v>
       </c>
@@ -19158,7 +19189,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="436" spans="1:12">
+    <row r="436" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A436" t="s">
         <v>434</v>
       </c>
@@ -19196,7 +19227,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="437" spans="1:12">
+    <row r="437" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A437" t="s">
         <v>435</v>
       </c>
@@ -19234,7 +19265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="438" spans="1:12">
+    <row r="438" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A438" t="s">
         <v>436</v>
       </c>
@@ -19272,7 +19303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="439" spans="1:12">
+    <row r="439" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A439" t="s">
         <v>437</v>
       </c>
@@ -19310,7 +19341,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="440" spans="1:12">
+    <row r="440" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A440" t="s">
         <v>438</v>
       </c>
@@ -19348,7 +19379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="441" spans="1:12">
+    <row r="441" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A441" t="s">
         <v>439</v>
       </c>
@@ -19383,7 +19414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="442" spans="1:12">
+    <row r="442" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A442" t="s">
         <v>440</v>
       </c>
@@ -19421,7 +19452,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="443" spans="1:12">
+    <row r="443" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A443" t="s">
         <v>441</v>
       </c>
@@ -19456,7 +19487,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="444" spans="1:12">
+    <row r="444" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A444" t="s">
         <v>442</v>
       </c>
@@ -19491,7 +19522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="445" spans="1:12">
+    <row r="445" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A445" t="s">
         <v>443</v>
       </c>
@@ -19529,7 +19560,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="446" spans="1:12">
+    <row r="446" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A446" t="s">
         <v>444</v>
       </c>
@@ -19567,7 +19598,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="447" spans="1:12">
+    <row r="447" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A447" t="s">
         <v>445</v>
       </c>
@@ -19605,7 +19636,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="448" spans="1:12">
+    <row r="448" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A448" t="s">
         <v>446</v>
       </c>
@@ -19643,7 +19674,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="449" spans="1:12">
+    <row r="449" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A449" t="s">
         <v>447</v>
       </c>
@@ -19681,7 +19712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="450" spans="1:12">
+    <row r="450" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A450" t="s">
         <v>448</v>
       </c>
@@ -19719,7 +19750,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="451" spans="1:12">
+    <row r="451" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A451" t="s">
         <v>449</v>
       </c>
@@ -19754,7 +19785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="452" spans="1:12">
+    <row r="452" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A452" t="s">
         <v>450</v>
       </c>
@@ -19792,7 +19823,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="453" spans="1:12">
+    <row r="453" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A453" t="s">
         <v>451</v>
       </c>
@@ -19830,7 +19861,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="454" spans="1:12">
+    <row r="454" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A454" t="s">
         <v>452</v>
       </c>
@@ -19868,7 +19899,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="455" spans="1:12">
+    <row r="455" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A455" t="s">
         <v>453</v>
       </c>
@@ -19903,7 +19934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="456" spans="1:12">
+    <row r="456" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A456" t="s">
         <v>454</v>
       </c>
@@ -19941,7 +19972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="457" spans="1:12">
+    <row r="457" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A457" t="s">
         <v>455</v>
       </c>
@@ -19979,7 +20010,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="458" spans="1:12">
+    <row r="458" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A458" t="s">
         <v>456</v>
       </c>
@@ -20017,7 +20048,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="459" spans="1:12">
+    <row r="459" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A459" t="s">
         <v>457</v>
       </c>
@@ -20055,7 +20086,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="460" spans="1:12">
+    <row r="460" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A460" t="s">
         <v>458</v>
       </c>
@@ -20090,7 +20121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="461" spans="1:12">
+    <row r="461" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A461" t="s">
         <v>459</v>
       </c>
@@ -20128,7 +20159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="462" spans="1:12">
+    <row r="462" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A462" t="s">
         <v>460</v>
       </c>
@@ -20166,7 +20197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="463" spans="1:12">
+    <row r="463" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A463" t="s">
         <v>461</v>
       </c>
@@ -20204,7 +20235,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="464" spans="1:12">
+    <row r="464" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A464" t="s">
         <v>462</v>
       </c>
@@ -20239,7 +20270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="465" spans="1:12">
+    <row r="465" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A465" t="s">
         <v>463</v>
       </c>
@@ -20277,7 +20308,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="466" spans="1:12">
+    <row r="466" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A466" t="s">
         <v>464</v>
       </c>
@@ -20315,7 +20346,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="467" spans="1:12">
+    <row r="467" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A467" t="s">
         <v>465</v>
       </c>
@@ -20353,7 +20384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="468" spans="1:12">
+    <row r="468" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A468" t="s">
         <v>466</v>
       </c>
@@ -20391,7 +20422,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="469" spans="1:12">
+    <row r="469" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A469" t="s">
         <v>467</v>
       </c>
@@ -20429,7 +20460,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="470" spans="1:12">
+    <row r="470" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A470" t="s">
         <v>468</v>
       </c>
@@ -20467,7 +20498,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="471" spans="1:12">
+    <row r="471" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A471" t="s">
         <v>469</v>
       </c>
@@ -20502,7 +20533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="472" spans="1:12">
+    <row r="472" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A472" t="s">
         <v>470</v>
       </c>
@@ -20537,7 +20568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="473" spans="1:12">
+    <row r="473" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A473" t="s">
         <v>471</v>
       </c>
@@ -20575,7 +20606,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="474" spans="1:12">
+    <row r="474" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A474" t="s">
         <v>472</v>
       </c>
@@ -20613,7 +20644,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="475" spans="1:12">
+    <row r="475" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A475" t="s">
         <v>473</v>
       </c>
@@ -20651,7 +20682,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="476" spans="1:12">
+    <row r="476" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A476" t="s">
         <v>474</v>
       </c>
@@ -20686,7 +20717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="477" spans="1:12">
+    <row r="477" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A477" t="s">
         <v>475</v>
       </c>
@@ -20721,7 +20752,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="478" spans="1:12">
+    <row r="478" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A478" t="s">
         <v>476</v>
       </c>
@@ -20759,7 +20790,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="479" spans="1:12">
+    <row r="479" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A479" t="s">
         <v>477</v>
       </c>
@@ -20797,7 +20828,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="480" spans="1:12">
+    <row r="480" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A480" t="s">
         <v>478</v>
       </c>
@@ -20835,7 +20866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="481" spans="1:12">
+    <row r="481" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A481" t="s">
         <v>479</v>
       </c>
@@ -20873,7 +20904,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="482" spans="1:12">
+    <row r="482" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A482" t="s">
         <v>480</v>
       </c>
@@ -20908,7 +20939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="483" spans="1:12">
+    <row r="483" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A483" t="s">
         <v>481</v>
       </c>
@@ -20946,7 +20977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="484" spans="1:12">
+    <row r="484" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A484" t="s">
         <v>482</v>
       </c>
@@ -20984,7 +21015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="485" spans="1:12">
+    <row r="485" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A485" t="s">
         <v>483</v>
       </c>
@@ -21022,7 +21053,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="486" spans="1:12">
+    <row r="486" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A486" t="s">
         <v>484</v>
       </c>
@@ -21057,7 +21088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="487" spans="1:12">
+    <row r="487" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A487" t="s">
         <v>485</v>
       </c>
@@ -21095,7 +21126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="488" spans="1:12">
+    <row r="488" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A488" t="s">
         <v>486</v>
       </c>
@@ -21133,7 +21164,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="489" spans="1:12">
+    <row r="489" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A489" t="s">
         <v>487</v>
       </c>
@@ -21171,7 +21202,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="490" spans="1:12">
+    <row r="490" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A490" t="s">
         <v>488</v>
       </c>
@@ -21206,7 +21237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="491" spans="1:12">
+    <row r="491" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A491" t="s">
         <v>489</v>
       </c>
@@ -21244,7 +21275,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="492" spans="1:12">
+    <row r="492" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A492" t="s">
         <v>490</v>
       </c>
@@ -21282,7 +21313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="493" spans="1:12">
+    <row r="493" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A493" t="s">
         <v>491</v>
       </c>
@@ -21320,7 +21351,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="494" spans="1:12">
+    <row r="494" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A494" t="s">
         <v>492</v>
       </c>
@@ -21355,7 +21386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="495" spans="1:12">
+    <row r="495" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A495" t="s">
         <v>493</v>
       </c>
@@ -21393,7 +21424,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="496" spans="1:12">
+    <row r="496" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A496" t="s">
         <v>494</v>
       </c>
@@ -21428,7 +21459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="497" spans="1:12">
+    <row r="497" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A497" t="s">
         <v>495</v>
       </c>
@@ -21466,7 +21497,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="498" spans="1:12">
+    <row r="498" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A498" t="s">
         <v>496</v>
       </c>
@@ -21504,7 +21535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="499" spans="1:12">
+    <row r="499" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A499" t="s">
         <v>497</v>
       </c>
@@ -21542,7 +21573,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="500" spans="1:12">
+    <row r="500" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A500" t="s">
         <v>498</v>
       </c>
@@ -21580,7 +21611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="501" spans="1:12">
+    <row r="501" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A501" t="s">
         <v>499</v>
       </c>
@@ -21618,7 +21649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="502" spans="1:12">
+    <row r="502" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A502" t="s">
         <v>500</v>
       </c>
@@ -21656,7 +21687,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="503" spans="1:12">
+    <row r="503" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A503" t="s">
         <v>501</v>
       </c>
@@ -21694,7 +21725,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="504" spans="1:12">
+    <row r="504" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A504" t="s">
         <v>502</v>
       </c>
@@ -21732,7 +21763,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="505" spans="1:12">
+    <row r="505" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A505" t="s">
         <v>503</v>
       </c>
@@ -21767,7 +21798,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="506" spans="1:12">
+    <row r="506" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A506" t="s">
         <v>504</v>
       </c>
@@ -21805,7 +21836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="507" spans="1:12">
+    <row r="507" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A507" t="s">
         <v>505</v>
       </c>
@@ -21843,7 +21874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="508" spans="1:12">
+    <row r="508" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A508" t="s">
         <v>506</v>
       </c>
@@ -21881,7 +21912,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="509" spans="1:12">
+    <row r="509" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A509" t="s">
         <v>507</v>
       </c>
@@ -21916,7 +21947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="510" spans="1:12">
+    <row r="510" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A510" t="s">
         <v>508</v>
       </c>
@@ -21951,7 +21982,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="511" spans="1:12">
+    <row r="511" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A511" t="s">
         <v>509</v>
       </c>
@@ -21989,7 +22020,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="512" spans="1:12">
+    <row r="512" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A512" t="s">
         <v>510</v>
       </c>
@@ -22027,7 +22058,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="513" spans="1:12">
+    <row r="513" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A513" t="s">
         <v>511</v>
       </c>
@@ -22065,7 +22096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="514" spans="1:12">
+    <row r="514" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A514" t="s">
         <v>512</v>
       </c>
@@ -22103,7 +22134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="515" spans="1:12">
+    <row r="515" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A515" t="s">
         <v>513</v>
       </c>
@@ -22141,7 +22172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="516" spans="1:12">
+    <row r="516" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A516" t="s">
         <v>514</v>
       </c>

</xml_diff>